<commit_message>
Commit - All done
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -3,22 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA4333F-66AB-435D-B5C8-6A2EE0B6638F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2786F5-640E-4DB0-A5B8-049024F06190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Page" sheetId="1" r:id="rId1"/>
-    <sheet name="Selected Vehicle Page" sheetId="2" r:id="rId2"/>
-    <sheet name="Book Service" sheetId="3" r:id="rId3"/>
+    <sheet name="OTP Page" sheetId="9" r:id="rId2"/>
+    <sheet name="Selected Vehicle Page" sheetId="2" r:id="rId3"/>
     <sheet name="My Profile" sheetId="5" r:id="rId4"/>
+    <sheet name="Emergency_contact" sheetId="6" r:id="rId5"/>
+    <sheet name="Book Service" sheetId="7" r:id="rId6"/>
+    <sheet name="Goodlife" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="97">
   <si>
     <t>8800996793</t>
   </si>
@@ -26,18 +29,9 @@
     <t>995859</t>
   </si>
   <si>
-    <t>Goodlife nonmem</t>
-  </si>
-  <si>
     <t>Book service FSC</t>
   </si>
   <si>
-    <t>2537461015</t>
-  </si>
-  <si>
-    <t>8800996794</t>
-  </si>
-  <si>
     <t>Valid mob number</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
     <t>110091</t>
   </si>
   <si>
-    <t>01-02-2023</t>
-  </si>
-  <si>
     <t>Invalid Full Name</t>
   </si>
   <si>
@@ -98,10 +89,235 @@
     <t>ABCD</t>
   </si>
   <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>f30, mumbai, bandra east +++++++@#%^^&amp;%^*!@#$@#$%^*^(</t>
+    <t>Valid_fullName</t>
+  </si>
+  <si>
+    <t>Valid_mobNumber</t>
+  </si>
+  <si>
+    <t>Valid_relationType</t>
+  </si>
+  <si>
+    <t>Invalid_fullName</t>
+  </si>
+  <si>
+    <t>Invalid_mobNumber</t>
+  </si>
+  <si>
+    <t>Invalid_relationType</t>
+  </si>
+  <si>
+    <t>Me</t>
+  </si>
+  <si>
+    <t>Friend</t>
+  </si>
+  <si>
+    <t>880099</t>
+  </si>
+  <si>
+    <t>Valid Emergency_Contacts_details</t>
+  </si>
+  <si>
+    <t>Invalid Emergency_Contacts_details</t>
+  </si>
+  <si>
+    <t>8809967681</t>
+  </si>
+  <si>
+    <t>Valid Book service details</t>
+  </si>
+  <si>
+    <t>Other's issues</t>
+  </si>
+  <si>
+    <t>Invalid Book service details</t>
+  </si>
+  <si>
+    <t>asdanskdajskdamskdnaskdnkwanknaskdnasndmasndn cxjaosduowquehjasnbdasjdkajskdajieuwiruweiruwiejdkasdkjasldkjowaieowqieorieirhaskjndasndknaskdjkajsdiwqueijwqekrjksabdkasnbdjasdjahsjdhoiwqueieuwqriyewriyweirjksnamdndmxz bcnzxb cnznbksjdakjwiuweiruohjaksdaksdkahsdkjawiehyrwiuehruiwerjwheriuweroiwqiehjqw</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;
+          &lt;h1&gt;Recent users queries:&lt;/h1&gt;
+          &lt;ol&gt;
+               &lt;li&gt;&lt;h2&gt;{user-query-1}&lt;/h2&gt; 
+               &lt;li&gt;&lt;h2&gt;{user-query-2}&lt;/h2&gt;
+         &lt;/ol&gt;
+      &lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>NomineeName</t>
+  </si>
+  <si>
+    <t>Karan</t>
+  </si>
+  <si>
+    <t>NomineeContactNumber</t>
+  </si>
+  <si>
+    <t>8130998133</t>
+  </si>
+  <si>
+    <t>RelativeName</t>
+  </si>
+  <si>
+    <t>Goodlife (Valid Insurance Page Details)</t>
+  </si>
+  <si>
+    <t>Goodlife (Invalid Insurance Page Details)</t>
+  </si>
+  <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>Karan1231239839172381aksdjkasjdaks#$%#&amp;</t>
+  </si>
+  <si>
+    <t>abcdef</t>
+  </si>
+  <si>
+    <t>ASDASDAJSDKNQEJ@#$$^%^%$%&amp;^%ADLKASDMASMD#@$#@%@^$%^%$&amp;^^%MSDFKSDF</t>
+  </si>
+  <si>
+    <t>abcd123&amp;#*$()</t>
+  </si>
+  <si>
+    <t>000000</t>
+  </si>
+  <si>
+    <t>f30mumbaibandraeast+++++++@#%^^&amp;%^*!@#$@#$%^*^(</t>
+  </si>
+  <si>
+    <t>2537461014</t>
+  </si>
+  <si>
+    <t>Mobile numbers</t>
+  </si>
+  <si>
+    <t>Login ( Expected results )</t>
+  </si>
+  <si>
+    <t>assertion_of_valid_login</t>
+  </si>
+  <si>
+    <t>assertion_of_invalid_login</t>
+  </si>
+  <si>
+    <t>Mobile Number is not registered</t>
+  </si>
+  <si>
+    <t>assertion_of_common_inLogin_page</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Vehicle Nickname</t>
+  </si>
+  <si>
+    <t>Vehicle Nickname's</t>
+  </si>
+  <si>
+    <t>Book service PAID</t>
+  </si>
+  <si>
+    <t>Verify with OTP</t>
+  </si>
+  <si>
+    <t>OTP (Expected results)</t>
+  </si>
+  <si>
+    <t>assertion_invalid_OTP</t>
+  </si>
+  <si>
+    <t>Invalid Otp</t>
+  </si>
+  <si>
+    <t>assertion_valid_OTP_with_no_internet</t>
+  </si>
+  <si>
+    <t>Please check your network connection.</t>
+  </si>
+  <si>
+    <t>1/2/23</t>
+  </si>
+  <si>
+    <t>1/2/01</t>
+  </si>
+  <si>
+    <t>Personal vaild details (Under my profile)</t>
+  </si>
+  <si>
+    <t>Personal invaild details (Under my profile)</t>
+  </si>
+  <si>
+    <t>Personal details page (Expected results)</t>
+  </si>
+  <si>
+    <t>validation_of_blank_fullName_field</t>
+  </si>
+  <si>
+    <t>validation_of_enter_invalid_email_field</t>
+  </si>
+  <si>
+    <t>validation_of_saving_without_internet</t>
+  </si>
+  <si>
+    <t>validation_of_invalid_date</t>
+  </si>
+  <si>
+    <t>validation_of_address</t>
+  </si>
+  <si>
+    <t>validation_of_invalid_pincode</t>
+  </si>
+  <si>
+    <t>gunjanrawat003@gmail.com</t>
+  </si>
+  <si>
+    <t>Age must be of 18yr old</t>
+  </si>
+  <si>
+    <t>f30mumbaibandraeast</t>
+  </si>
+  <si>
+    <t>Not to able to get state and city from pincode</t>
+  </si>
+  <si>
+    <t>Valid saved contact number</t>
+  </si>
+  <si>
+    <t>Emergency contact page (Expected results)</t>
+  </si>
+  <si>
+    <t>validation_of_deleting_contact</t>
+  </si>
+  <si>
+    <t>Add Emergency contact</t>
+  </si>
+  <si>
+    <t>assertion_of_already_exist_contact</t>
+  </si>
+  <si>
+    <t>This Emergency Contact Already Exists</t>
+  </si>
+  <si>
+    <t>validation_of_invalid_fullName</t>
+  </si>
+  <si>
+    <t>abcd123</t>
+  </si>
+  <si>
+    <t>Validation_of_saving_blank_and_invalid_field</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Relation Type</t>
+  </si>
+  <si>
+    <t>validation_saving_with_no_internet</t>
   </si>
 </sst>
 </file>
@@ -117,16 +333,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -135,18 +341,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
-      <color rgb="FF2A00FF"/>
+      <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -160,20 +387,36 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -514,7 +757,538 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="40" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="8"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A11:B11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D31A8F-3FBA-4F47-85D0-BA6DBB6214F8}">
+  <dimension ref="A8:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="39.08984375" customWidth="1"/>
+    <col min="2" max="2" width="47" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:B8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="38.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A11:B11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="48.6328125" customWidth="1"/>
+    <col min="2" max="2" width="52.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A24:B24"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{AC2E004A-B721-44EF-A519-77594C330DB5}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{1E98206A-73D5-4A8D-94B1-7EF178E5E015}"/>
+    <hyperlink ref="B17" r:id="rId3" xr:uid="{1526CF94-F6A9-4F64-9F94-C88E5E5C3A03}"/>
+    <hyperlink ref="B26" r:id="rId4" xr:uid="{559745FE-7564-41C2-9E82-584DD90D55A4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC974FB1-DE16-4A47-8399-1BAE83A3EDA8}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="46.90625" customWidth="1"/>
+    <col min="2" max="2" width="53" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="9"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A19:B19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CDB8472-B486-47FF-A7BC-EA275ED1BDE9}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -522,199 +1296,131 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.54296875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="45.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
+      <c r="A1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A8:B8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A3"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6CCBC5-1399-4ECF-9AF6-16C29B60B677}">
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="34.453125" customWidth="1"/>
+    <col min="2" max="2" width="38.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="16.1796875" customWidth="1"/>
-    <col min="2" max="2" width="57.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="A1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="9"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>18</v>
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>18</v>
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
+      <c r="A11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="9"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A11:B11"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{86BA8BCA-8DBA-4CBE-A7EB-756739F75076}"/>
-    <hyperlink ref="B8" r:id="rId2" xr:uid="{0845EB4D-D4B2-4E47-A392-66DCDC5D0744}"/>
+    <hyperlink ref="B15" r:id="rId1" xr:uid="{F36C9C6B-09C5-44E8-8D59-F487BC8D988E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
I have added latest build with Updated test cases
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBE1E6E-1C38-475D-BA5A-013675561759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159F7B1F-4C2B-485C-B701-7DE86CAEA756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Page" sheetId="1" r:id="rId1"/>
@@ -179,145 +179,145 @@
     <t>abcd123&amp;#*$()</t>
   </si>
   <si>
+    <t>f30mumbaibandraeast+++++++@#%^^&amp;%^*!@#$@#$%^*^(</t>
+  </si>
+  <si>
+    <t>2537461014</t>
+  </si>
+  <si>
+    <t>Mobile numbers</t>
+  </si>
+  <si>
+    <t>Login ( Expected results )</t>
+  </si>
+  <si>
+    <t>assertion_of_valid_login</t>
+  </si>
+  <si>
+    <t>assertion_of_invalid_login</t>
+  </si>
+  <si>
+    <t>Mobile Number is not registered</t>
+  </si>
+  <si>
+    <t>assertion_of_common_inLogin_page</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Vehicle Nickname</t>
+  </si>
+  <si>
+    <t>Vehicle Nickname's</t>
+  </si>
+  <si>
+    <t>Book service PAID</t>
+  </si>
+  <si>
+    <t>Verify with OTP</t>
+  </si>
+  <si>
+    <t>OTP (Expected results)</t>
+  </si>
+  <si>
+    <t>assertion_invalid_OTP</t>
+  </si>
+  <si>
+    <t>assertion_valid_OTP_with_no_internet</t>
+  </si>
+  <si>
+    <t>Please check your network connection.</t>
+  </si>
+  <si>
+    <t>1/2/23</t>
+  </si>
+  <si>
+    <t>1/2/01</t>
+  </si>
+  <si>
+    <t>Personal vaild details (Under my profile)</t>
+  </si>
+  <si>
+    <t>Personal invaild details (Under my profile)</t>
+  </si>
+  <si>
+    <t>Personal details page (Expected results)</t>
+  </si>
+  <si>
+    <t>validation_of_blank_fullName_field</t>
+  </si>
+  <si>
+    <t>validation_of_enter_invalid_email_field</t>
+  </si>
+  <si>
+    <t>validation_of_saving_without_internet</t>
+  </si>
+  <si>
+    <t>validation_of_invalid_date</t>
+  </si>
+  <si>
+    <t>validation_of_address</t>
+  </si>
+  <si>
+    <t>validation_of_invalid_pincode</t>
+  </si>
+  <si>
+    <t>gunjanrawat003@gmail.com</t>
+  </si>
+  <si>
+    <t>Age must be of 18yr old</t>
+  </si>
+  <si>
+    <t>f30mumbaibandraeast</t>
+  </si>
+  <si>
+    <t>Valid saved contact number</t>
+  </si>
+  <si>
+    <t>Emergency contact page (Expected results)</t>
+  </si>
+  <si>
+    <t>validation_of_deleting_contact</t>
+  </si>
+  <si>
+    <t>Add Emergency contact</t>
+  </si>
+  <si>
+    <t>assertion_of_already_exist_contact</t>
+  </si>
+  <si>
+    <t>This Emergency Contact Already Exists</t>
+  </si>
+  <si>
+    <t>validation_of_invalid_fullName</t>
+  </si>
+  <si>
+    <t>abcd123</t>
+  </si>
+  <si>
+    <t>Validation_of_saving_blank_and_invalid_field</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Relation Type</t>
+  </si>
+  <si>
+    <t>validation_saving_with_no_internet</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>9958592171</t>
+  </si>
+  <si>
+    <t>PIN Code</t>
+  </si>
+  <si>
     <t>000000</t>
-  </si>
-  <si>
-    <t>f30mumbaibandraeast+++++++@#%^^&amp;%^*!@#$@#$%^*^(</t>
-  </si>
-  <si>
-    <t>2537461014</t>
-  </si>
-  <si>
-    <t>Mobile numbers</t>
-  </si>
-  <si>
-    <t>Login ( Expected results )</t>
-  </si>
-  <si>
-    <t>assertion_of_valid_login</t>
-  </si>
-  <si>
-    <t>assertion_of_invalid_login</t>
-  </si>
-  <si>
-    <t>Mobile Number is not registered</t>
-  </si>
-  <si>
-    <t>assertion_of_common_inLogin_page</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Vehicle Nickname</t>
-  </si>
-  <si>
-    <t>Vehicle Nickname's</t>
-  </si>
-  <si>
-    <t>Book service PAID</t>
-  </si>
-  <si>
-    <t>Verify with OTP</t>
-  </si>
-  <si>
-    <t>OTP (Expected results)</t>
-  </si>
-  <si>
-    <t>assertion_invalid_OTP</t>
-  </si>
-  <si>
-    <t>assertion_valid_OTP_with_no_internet</t>
-  </si>
-  <si>
-    <t>Please check your network connection.</t>
-  </si>
-  <si>
-    <t>1/2/23</t>
-  </si>
-  <si>
-    <t>1/2/01</t>
-  </si>
-  <si>
-    <t>Personal vaild details (Under my profile)</t>
-  </si>
-  <si>
-    <t>Personal invaild details (Under my profile)</t>
-  </si>
-  <si>
-    <t>Personal details page (Expected results)</t>
-  </si>
-  <si>
-    <t>validation_of_blank_fullName_field</t>
-  </si>
-  <si>
-    <t>validation_of_enter_invalid_email_field</t>
-  </si>
-  <si>
-    <t>validation_of_saving_without_internet</t>
-  </si>
-  <si>
-    <t>validation_of_invalid_date</t>
-  </si>
-  <si>
-    <t>validation_of_address</t>
-  </si>
-  <si>
-    <t>validation_of_invalid_pincode</t>
-  </si>
-  <si>
-    <t>gunjanrawat003@gmail.com</t>
-  </si>
-  <si>
-    <t>Age must be of 18yr old</t>
-  </si>
-  <si>
-    <t>f30mumbaibandraeast</t>
-  </si>
-  <si>
-    <t>Not to able to get state and city from pincode</t>
-  </si>
-  <si>
-    <t>Valid saved contact number</t>
-  </si>
-  <si>
-    <t>Emergency contact page (Expected results)</t>
-  </si>
-  <si>
-    <t>validation_of_deleting_contact</t>
-  </si>
-  <si>
-    <t>Add Emergency contact</t>
-  </si>
-  <si>
-    <t>assertion_of_already_exist_contact</t>
-  </si>
-  <si>
-    <t>This Emergency Contact Already Exists</t>
-  </si>
-  <si>
-    <t>validation_of_invalid_fullName</t>
-  </si>
-  <si>
-    <t>abcd123</t>
-  </si>
-  <si>
-    <t>Validation_of_saving_blank_and_invalid_field</t>
-  </si>
-  <si>
-    <t>Full Name</t>
-  </si>
-  <si>
-    <t>Relation Type</t>
-  </si>
-  <si>
-    <t>validation_saving_with_no_internet</t>
-  </si>
-  <si>
-    <t>Save</t>
-  </si>
-  <si>
-    <t>9958592171</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -405,6 +405,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -759,7 +762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -770,17 +773,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="8"/>
+      <c r="A1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -788,7 +791,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -807,33 +810,33 @@
       <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="8"/>
+      <c r="A11" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="9"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
         <v>56</v>
-      </c>
-      <c r="B13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
         <v>58</v>
-      </c>
-      <c r="B14" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -864,25 +867,25 @@
   </cols>
   <sheetData>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="9"/>
+      <c r="A8" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="10"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
         <v>66</v>
-      </c>
-      <c r="B10" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -909,30 +912,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="8"/>
+      <c r="A1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -947,7 +950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -958,10 +961,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="9"/>
+      <c r="A1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -984,7 +987,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1016,10 +1019,10 @@
       <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="9"/>
+      <c r="A13" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="10"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1042,7 +1045,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -1050,15 +1053,15 @@
         <v>17</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>50</v>
+      <c r="B18" s="8" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1074,14 +1077,14 @@
       <c r="B23" s="1"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" s="9"/>
+      <c r="A24" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="10"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -1089,42 +1092,42 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1160,10 +1163,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1191,17 +1194,17 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="9"/>
+      <c r="B9" s="10"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1224,45 +1227,45 @@
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19" s="9"/>
+      <c r="A19" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="10"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -1270,10 +1273,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1301,10 +1304,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1315,10 +1318,10 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="9"/>
+      <c r="B8" s="10"/>
     </row>
     <row r="9" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -1343,7 +1346,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1353,10 +1356,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -1383,10 +1386,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="9"/>
+      <c r="B11" s="10"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">

</xml_diff>

<commit_message>
Added new build. Added Goodlife membership cases.
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159F7B1F-4C2B-485C-B701-7DE86CAEA756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0709B19-6B38-4A8D-8E74-FD6F8B08F20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Page" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="100">
   <si>
     <t>995859</t>
-  </si>
-  <si>
-    <t>Book service FSC</t>
   </si>
   <si>
     <t>Valid mob number</t>
@@ -206,9 +203,6 @@
     <t>Login</t>
   </si>
   <si>
-    <t>Vehicle Nickname</t>
-  </si>
-  <si>
     <t>Vehicle Nickname's</t>
   </si>
   <si>
@@ -318,6 +312,21 @@
   </si>
   <si>
     <t>000000</t>
+  </si>
+  <si>
+    <t>7777700189</t>
+  </si>
+  <si>
+    <t>Goodlife Member</t>
+  </si>
+  <si>
+    <t>Goodlife member mob number</t>
+  </si>
+  <si>
+    <t>Vehicle Nickname1</t>
+  </si>
+  <si>
+    <t>Vehicle Nickname2</t>
   </si>
 </sst>
 </file>
@@ -763,7 +772,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -774,36 +783,41 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
@@ -811,32 +825,32 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="9"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
         <v>55</v>
-      </c>
-      <c r="B13" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
         <v>57</v>
-      </c>
-      <c r="B14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -868,24 +882,24 @@
   <sheetData>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="10"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -901,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -913,24 +927,24 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -950,7 +964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -962,48 +976,48 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1020,48 +1034,48 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B13" s="10"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1078,56 +1092,56 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B24" s="10"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1164,108 +1178,108 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="10"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B19" s="10"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -1273,10 +1287,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1305,30 +1319,30 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="10"/>
     </row>
     <row r="9" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1357,62 +1371,62 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
         <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="10"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I have created interface and changed the classes as well with new application also added
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0709B19-6B38-4A8D-8E74-FD6F8B08F20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E6435A-3EFC-42E7-A5AE-8395464C3430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Page" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="Emergency_contact" sheetId="6" r:id="rId5"/>
     <sheet name="Book Service" sheetId="7" r:id="rId6"/>
     <sheet name="Goodlife" sheetId="8" r:id="rId7"/>
+    <sheet name="Goodlife Member" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="92">
   <si>
     <t>995859</t>
   </si>
@@ -185,42 +186,9 @@
     <t>Mobile numbers</t>
   </si>
   <si>
-    <t>Login ( Expected results )</t>
-  </si>
-  <si>
-    <t>assertion_of_valid_login</t>
-  </si>
-  <si>
-    <t>assertion_of_invalid_login</t>
-  </si>
-  <si>
-    <t>Mobile Number is not registered</t>
-  </si>
-  <si>
-    <t>assertion_of_common_inLogin_page</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
     <t>Vehicle Nickname's</t>
   </si>
   <si>
-    <t>Book service PAID</t>
-  </si>
-  <si>
-    <t>Verify with OTP</t>
-  </si>
-  <si>
-    <t>OTP (Expected results)</t>
-  </si>
-  <si>
-    <t>assertion_invalid_OTP</t>
-  </si>
-  <si>
-    <t>assertion_valid_OTP_with_no_internet</t>
-  </si>
-  <si>
     <t>Please check your network connection.</t>
   </si>
   <si>
@@ -314,12 +282,6 @@
     <t>000000</t>
   </si>
   <si>
-    <t>7777700189</t>
-  </si>
-  <si>
-    <t>Goodlife Member</t>
-  </si>
-  <si>
     <t>Goodlife member mob number</t>
   </si>
   <si>
@@ -327,6 +289,21 @@
   </si>
   <si>
     <t>Vehicle Nickname2</t>
+  </si>
+  <si>
+    <t>Goodlife Member Valid Details</t>
+  </si>
+  <si>
+    <t>Winner Of The Month</t>
+  </si>
+  <si>
+    <t>MANISH VERMA</t>
+  </si>
+  <si>
+    <t>book service paid</t>
+  </si>
+  <si>
+    <t>goodlife member</t>
   </si>
 </sst>
 </file>
@@ -421,10 +398,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -769,16 +746,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="2" max="2" width="55" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -792,7 +769,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -813,10 +790,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -824,42 +801,11 @@
       <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="9"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B15" s="4"/>
+      <c r="B11" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -868,44 +814,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D31A8F-3FBA-4F47-85D0-BA6DBB6214F8}">
-  <dimension ref="A8:B10"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.08984375" customWidth="1"/>
-    <col min="2" max="2" width="47" customWidth="1"/>
+    <col min="1" max="1" width="39.08984375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="47" customWidth="1" collapsed="1"/>
   </cols>
-  <sheetData>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="10"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A8:B8"/>
-  </mergeCells>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -915,41 +835,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="38.26953125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.90625" customWidth="1"/>
+    <col min="2" max="2" width="44.90625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -964,21 +884,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="48.6328125" customWidth="1"/>
-    <col min="2" max="2" width="52.90625" customWidth="1"/>
+    <col min="1" max="1" width="48.6328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="52.90625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="10"/>
+      <c r="A1" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1001,7 +921,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1033,10 +953,10 @@
       <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="10"/>
+      <c r="A13" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="11"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1059,7 +979,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -1075,7 +995,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1091,14 +1011,14 @@
       <c r="B23" s="1"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="10"/>
+      <c r="A24" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="11"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
@@ -1106,42 +1026,42 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1171,16 +1091,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="46.90625" customWidth="1"/>
-    <col min="2" max="2" width="53" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="46.90625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1208,17 +1128,17 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="11"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1241,45 +1161,45 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="10"/>
+      <c r="A19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="11"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -1287,10 +1207,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1313,15 +1233,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="45.7265625" customWidth="1"/>
+    <col min="1" max="1" width="35" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.7265625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1335,7 +1255,7 @@
       <c r="A8" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="11"/>
     </row>
     <row r="9" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -1365,15 +1285,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.453125" customWidth="1"/>
-    <col min="2" max="2" width="38.6328125" customWidth="1"/>
+    <col min="1" max="1" width="34.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.6328125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -1400,10 +1320,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="10"/>
+      <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1440,4 +1360,41 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F17E65-FAAF-45A5-B8DE-BC6018B33B5D}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="40.6328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.54296875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TestCaseUpdated, config file , excel file - 26 July
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E550D5-9906-4424-866F-28FBFD388A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09A997D-434B-4234-9627-73331BA87B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -291,7 +291,7 @@
     <t>abcd123&amp;#*$()</t>
   </si>
   <si>
-    <t>7777777777</t>
+    <t>6666600022</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated Android Login, RM, TipsDIY PO and update test cases
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09A997D-434B-4234-9627-73331BA87B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D8D2B4-E9D0-4EF9-9A59-A5D76613E0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Page" sheetId="1" r:id="rId1"/>
-    <sheet name="OTP Page" sheetId="9" r:id="rId2"/>
-    <sheet name="Selected Vehicle Page" sheetId="2" r:id="rId3"/>
-    <sheet name="My Profile" sheetId="5" r:id="rId4"/>
-    <sheet name="Emergency_contact" sheetId="6" r:id="rId5"/>
+    <sheet name="Selected Vehicle Page" sheetId="2" r:id="rId2"/>
+    <sheet name="My Profile" sheetId="5" r:id="rId3"/>
+    <sheet name="Emergency_contact" sheetId="6" r:id="rId4"/>
+    <sheet name="Refer a friend" sheetId="11" r:id="rId5"/>
     <sheet name="Book Service" sheetId="7" r:id="rId6"/>
     <sheet name="Goodlife" sheetId="8" r:id="rId7"/>
     <sheet name="Goodlife Member" sheetId="10" r:id="rId8"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="107">
   <si>
     <t>995859</t>
   </si>
@@ -78,19 +78,10 @@
     <t>Valid_relationType</t>
   </si>
   <si>
-    <t>Invalid_mobNumber</t>
-  </si>
-  <si>
-    <t>Invalid_relationType</t>
-  </si>
-  <si>
     <t>Me</t>
   </si>
   <si>
     <t>Friend</t>
-  </si>
-  <si>
-    <t>880099</t>
   </si>
   <si>
     <t>Valid Emergency_Contacts_details</t>
@@ -177,9 +168,6 @@
     <t>Valid saved contact number</t>
   </si>
   <si>
-    <t>Relation Type</t>
-  </si>
-  <si>
     <t>9958592171</t>
   </si>
   <si>
@@ -285,13 +273,82 @@
     <t>Invalid Emergency_Contacts_details</t>
   </si>
   <si>
-    <t>Invalid_fullName</t>
-  </si>
-  <si>
-    <t>abcd123&amp;#*$()</t>
-  </si>
-  <si>
     <t>6666600022</t>
+  </si>
+  <si>
+    <t>110091++++++++++++@#%@#%#^$%&amp;&amp;)*)!#$!</t>
+  </si>
+  <si>
+    <t>&lt;/h2&gt;special offer &lt;a href=www.attacker.site&gt;malicious link&lt;/a&gt;&lt;h2&gt;</t>
+  </si>
+  <si>
+    <t>InValid FullName with HTMLINJECTIONS</t>
+  </si>
+  <si>
+    <t>InValid MobileNumber with Email</t>
+  </si>
+  <si>
+    <t>InValid MobileNumber with DOB</t>
+  </si>
+  <si>
+    <t>InValid MobileNumber with HTMLINJECTIONS</t>
+  </si>
+  <si>
+    <t>InValid MobileNumber with Pincode</t>
+  </si>
+  <si>
+    <t>Y+!@#$%^&amp;*()</t>
+  </si>
+  <si>
+    <t>InValid MobileNumber with AlphaNumeric</t>
+  </si>
+  <si>
+    <t>8123123Yes</t>
+  </si>
+  <si>
+    <t>Valid Refer a friend details</t>
+  </si>
+  <si>
+    <t>Valid_MobileNumber</t>
+  </si>
+  <si>
+    <t>Valid_Friend'sName</t>
+  </si>
+  <si>
+    <t>InValid Refer a friend details</t>
+  </si>
+  <si>
+    <t>MyName</t>
+  </si>
+  <si>
+    <t>InValid Friend'sName with Email</t>
+  </si>
+  <si>
+    <t>InValid Friend'sName with DOB</t>
+  </si>
+  <si>
+    <t>InValid Friend'sName with HTMLINJECTIONS</t>
+  </si>
+  <si>
+    <t>InValid Friend'sName with Pincode</t>
+  </si>
+  <si>
+    <t>Valid_State</t>
+  </si>
+  <si>
+    <t>Valid_City</t>
+  </si>
+  <si>
+    <t>Valid_ModelName</t>
+  </si>
+  <si>
+    <t>delhi</t>
+  </si>
+  <si>
+    <t>Destini 125</t>
+  </si>
+  <si>
+    <t>new delhi</t>
   </si>
 </sst>
 </file>
@@ -694,7 +751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -706,7 +763,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B1" s="9"/>
     </row>
@@ -715,7 +772,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -723,7 +780,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -736,10 +793,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -759,25 +816,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D31A8F-3FBA-4F47-85D0-BA6DBB6214F8}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="39.08984375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="47" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -793,24 +831,24 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -826,12 +864,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -842,7 +880,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B1" s="11"/>
     </row>
@@ -859,7 +897,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -906,7 +944,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>10</v>
@@ -914,15 +952,15 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>11</v>
@@ -930,7 +968,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>12</v>
@@ -959,15 +997,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>11</v>
@@ -975,26 +1013,26 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -1017,15 +1055,15 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>11</v>
@@ -1033,26 +1071,26 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -1072,7 +1110,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>13</v>
@@ -1080,7 +1118,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B46" t="s">
         <v>14</v>
@@ -1088,26 +1126,26 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -1139,24 +1177,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC974FB1-DE16-4A47-8399-1BAE83A3EDA8}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="46.90625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="53" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="69.81640625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B1" s="11"/>
     </row>
@@ -1165,7 +1203,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1173,7 +1211,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1181,61 +1219,96 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B9" s="11"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" t="s">
-        <v>86</v>
+        <v>69</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>70</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
+        <v>84</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>22</v>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>49</v>
+        <v>88</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1243,7 +1316,129 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A9:B9"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{5E64759D-E8FF-4C48-A0DE-E6DE01890F3F}"/>
+    <hyperlink ref="B18" r:id="rId2" display="gunjan007@gmail.com" xr:uid="{1EED5F04-4199-46F9-9362-A43E0793ABDE}"/>
+    <hyperlink ref="B21" r:id="rId3" xr:uid="{0A8A9558-F3D8-438C-9775-62E927769CC0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6AD3DBC-E355-41E0-8CA6-818EB8E40574}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="40.453125" customWidth="1"/>
+    <col min="2" max="2" width="62.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="11"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A10:B10"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{6DF8A508-2F17-4B0E-81CD-0ECC4C12286A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1263,30 +1458,30 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B8" s="11"/>
     </row>
     <row r="9" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1315,62 +1510,62 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
         <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1402,16 +1597,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest changes on 5 feb
Latest changes on 5 feb
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D8D2B4-E9D0-4EF9-9A59-A5D76613E0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DB16B6-F430-4D9B-B37C-65A21339C452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Page" sheetId="1" r:id="rId1"/>
@@ -273,9 +273,6 @@
     <t>Invalid Emergency_Contacts_details</t>
   </si>
   <si>
-    <t>6666600022</t>
-  </si>
-  <si>
     <t>110091++++++++++++@#%@#%#^$%&amp;&amp;)*)!#$!</t>
   </si>
   <si>
@@ -349,6 +346,9 @@
   </si>
   <si>
     <t>new delhi</t>
+  </si>
+  <si>
+    <t>8800996677</t>
   </si>
 </sst>
 </file>
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -772,7 +772,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1254,10 +1254,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -1265,7 +1265,7 @@
         <v>72</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -1273,7 +1273,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>14</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>43</v>
@@ -1289,26 +1289,26 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" t="s">
         <v>90</v>
-      </c>
-      <c r="B22" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1329,7 +1329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6AD3DBC-E355-41E0-8CA6-818EB8E40574}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1341,21 +1341,21 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
@@ -1363,26 +1363,26 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1393,13 +1393,13 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>43</v>
@@ -1415,18 +1415,18 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>